<commit_message>
Added my team member folder and all the use-case related deliveries from my contributions, waiting for peer reviewing. Also fixed some xls formatting and typos.
</commit_message>
<xml_diff>
--- a/Project/Phase_1/Sprint_1/Burndown Chart.xlsx
+++ b/Project/Phase_1/Sprint_1/Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\JabRef\jabref\Project\Phase_1\Sprint_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67081D28-C67F-4B51-AD1D-3202028D4D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E1A9D-E1A6-408E-B623-BE08AA6B1A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="6570" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Burndown Chart" sheetId="6" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -104,13 +104,7 @@
     <t xml:space="preserve">Week </t>
   </si>
   <si>
-    <t>Team Oracle</t>
-  </si>
-  <si>
     <t>Day</t>
-  </si>
-  <si>
-    <t>This sheet is meant to describe one sprint (per phase)</t>
   </si>
   <si>
     <t>THE SPRINT BURNDOWN CHART</t>
@@ -131,9 +125,6 @@
     <t>Average Work / Day</t>
   </si>
   <si>
-    <t>* You only use this chart for the tasks in the backlog and that will be achieved in the sprint, non management tasks. For example, related to modelling the system in Papyrus, OCL in USE, or detailed description of the Use Cases using the doc templates, analysis of the Uber website etc</t>
-  </si>
-  <si>
     <t>Actual Work</t>
   </si>
   <si>
@@ -147,15 +138,6 @@
   </si>
   <si>
     <t>Ideal Work Remaining</t>
-  </si>
-  <si>
-    <t>The Ideal backlog remaining should be a straight line</t>
-  </si>
-  <si>
-    <t>To fill in the Done column you should insert the hours with work done according to the estimated hours per task in the Backlog</t>
-  </si>
-  <si>
-    <t>The sprint has a fixed duration. Fill in the table below the exact number of days, instead of 30, and adapt the formulas accordingly.</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1242,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1291,25 +1273,21 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="H2" s="17" t="s">
-        <v>3</v>
-      </c>
+      <c r="H2" s="17"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="8"/>
       <c r="B4" s="3"/>
       <c r="C4" s="16"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1322,11 +1300,11 @@
       <c r="B7" s="12"/>
       <c r="C7" s="9"/>
       <c r="E7" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="10"/>
       <c r="H7" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I7" s="19"/>
     </row>
@@ -1335,27 +1313,25 @@
       <c r="B8" s="12"/>
       <c r="C8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I8" s="11">
         <f>ROUND(F8/A22,1)</f>
         <v>0</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F9" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1367,7 +1343,7 @@
     </row>
     <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="21"/>
       <c r="E10" s="5">
@@ -1377,23 +1353,21 @@
     </row>
     <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="G11" s="8"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
@@ -1411,9 +1385,7 @@
         <f>F8</f>
         <v>0</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="G12" s="8"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1976,9 +1948,7 @@
       <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>

</xml_diff>

<commit_message>
Updated Burndown Chart xls
</commit_message>
<xml_diff>
--- a/Project/Phase_1/Sprint_1/Burndown Chart.xlsx
+++ b/Project/Phase_1/Sprint_1/Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\JabRef\jabref\Project\Phase_1\Sprint_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E1A9D-E1A6-408E-B623-BE08AA6B1A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD48ADE8-5133-403A-BD4A-F2A447A273CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="6570" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Burndown Chart" sheetId="6" r:id="rId1"/>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -188,9 +188,17 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -280,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyAlignment="1">
@@ -303,12 +311,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,91 +502,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -714,94 +721,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>54.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>52.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>50.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>49.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>47.300000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>45.500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>43.700000000000017</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>41.90000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>40.100000000000023</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>38.300000000000026</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>36.500000000000028</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>34.700000000000031</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>32.900000000000034</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>31.100000000000033</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>29.300000000000033</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>27.500000000000032</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>25.700000000000031</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>23.900000000000031</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>22.10000000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>20.300000000000029</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>18.500000000000028</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>16.700000000000028</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>14.900000000000027</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>13.100000000000026</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>11.300000000000026</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>9.5000000000000249</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>7.700000000000025</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>5.9000000000000252</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>4.1000000000000254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,7 +1249,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1258,34 +1265,34 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
-      <c r="H1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="19">
+        <v>44536</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="13">
+        <v>3</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="13">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="H2" s="17"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="15"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
@@ -1302,11 +1309,15 @@
       <c r="E7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="20">
+        <v>44536</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
@@ -1315,7 +1326,9 @@
       <c r="E8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="14">
+        <v>60</v>
+      </c>
       <c r="G8" s="13" t="s">
         <v>8</v>
       </c>
@@ -1324,7 +1337,7 @@
       </c>
       <c r="I8" s="11">
         <f>ROUND(F8/A22,1)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>8</v>
@@ -1342,13 +1355,13 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="18"/>
       <c r="E10" s="5">
         <f>ROUND(C41/29,1)</f>
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
@@ -1375,15 +1388,19 @@
       <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
       <c r="D12" s="5">
-        <f t="shared" ref="D12:D41" si="0">$C$41-C12</f>
-        <v>0</v>
+        <f>$C$41-C12</f>
+        <v>53</v>
       </c>
       <c r="E12" s="5">
         <f>F8</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
@@ -1395,553 +1412,611 @@
     </row>
     <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <f t="shared" ref="A13:A41" si="1">A12+1</f>
+        <f t="shared" ref="A13:A41" si="0">A12+1</f>
         <v>2</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
       <c r="C13" s="6">
-        <f t="shared" ref="C13:C41" si="2">B13+C12</f>
+        <f t="shared" ref="C13:C41" si="1">B13+C12</f>
         <v>0</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>$C$41-C13</f>
+        <v>53</v>
       </c>
       <c r="E13" s="5">
         <f>E12-$I$8</f>
-        <v>0</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
       <c r="C14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D12:D41" si="2">$C$41-C14</f>
+        <v>53</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" ref="E14:E41" si="3">E13-$E$10</f>
-        <v>0</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
       <c r="C15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>50.900000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
       <c r="C16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>49.100000000000009</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
       <c r="C17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>47.300000000000011</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
       <c r="C18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45.500000000000014</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
       <c r="C19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>43.700000000000017</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
       <c r="C20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>41.90000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
       <c r="C21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40.100000000000023</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
       <c r="C22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>38.300000000000026</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
       <c r="C23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>36.500000000000028</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
       <c r="C24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>34.700000000000031</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
       <c r="C25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>32.900000000000034</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
       <c r="C26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E26" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>31.100000000000033</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
       <c r="C27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>29.300000000000033</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
       <c r="C28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E28" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27.500000000000032</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
       <c r="C29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>25.700000000000031</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
       <c r="C30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E30" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23.900000000000031</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
       <c r="C31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E31" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>22.10000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
       <c r="C32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20.300000000000029</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B33" s="6"/>
+      <c r="B33" s="6">
+        <v>5</v>
+      </c>
       <c r="C33" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="D33" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
       <c r="E33" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>18.500000000000028</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="6">
+        <v>10</v>
+      </c>
       <c r="C34" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="E34" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>16.700000000000028</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B35" s="6"/>
+      <c r="B35" s="6">
+        <v>4</v>
+      </c>
       <c r="C35" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.900000000000027</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B36" s="6"/>
+      <c r="B36" s="6">
+        <v>3</v>
+      </c>
       <c r="C36" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>13.100000000000026</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B37" s="6"/>
+      <c r="B37" s="6">
+        <v>4</v>
+      </c>
       <c r="C37" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11.300000000000026</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="6">
+        <v>4</v>
+      </c>
       <c r="C38" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="E38" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.5000000000000249</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="6">
+        <v>10</v>
+      </c>
       <c r="C39" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="E39" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.700000000000025</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B40" s="6"/>
+      <c r="B40" s="6">
+        <v>8</v>
+      </c>
       <c r="C40" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>48</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="E40" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.9000000000000252</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B41" s="6"/>
+      <c r="B41" s="6">
+        <v>5</v>
+      </c>
       <c r="C41" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>53</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E41" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.1000000000000254</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>